<commit_message>
#Modificación de permisos terminado
</commit_message>
<xml_diff>
--- a/Anotaciones/FamiliasYPatentes.xlsx
+++ b/Anotaciones/FamiliasYPatentes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>ABM Solicitud</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>Crear Partida</t>
+  </si>
+  <si>
+    <t>Modificar Partida</t>
   </si>
 </sst>
 </file>
@@ -84,7 +90,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,27 +146,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -437,9 +453,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H6:O14"/>
+  <dimension ref="H6:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -451,28 +467,28 @@
   </cols>
   <sheetData>
     <row r="6" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="2"/>
+      <c r="N6" s="7"/>
     </row>
     <row r="7" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="7"/>
       <c r="M7" s="1">
         <v>1</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="8:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>1</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" t="s">
@@ -481,7 +497,7 @@
       <c r="M8" s="1">
         <v>2</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -489,13 +505,13 @@
       <c r="H9" s="1">
         <v>2</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="9" t="s">
         <v>1</v>
       </c>
       <c r="M9" s="1">
         <v>3</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -503,7 +519,7 @@
       <c r="H10" s="1">
         <v>3</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>2</v>
       </c>
       <c r="J10" t="s">
@@ -520,16 +536,16 @@
       </c>
     </row>
     <row r="11" spans="8:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>4</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="M11" s="1">
         <v>5</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="N11" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -537,7 +553,7 @@
       <c r="M12" s="1">
         <v>6</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -545,7 +561,7 @@
       <c r="M13" s="1">
         <v>7</v>
       </c>
-      <c r="N13" s="7" t="s">
+      <c r="N13" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -553,8 +569,24 @@
       <c r="M14" s="1">
         <v>8</v>
       </c>
-      <c r="N14" s="7" t="s">
+      <c r="N14" s="6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M15" s="1">
+        <v>9</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="M16" s="1">
+        <v>10</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>